<commit_message>
in lasta date estimate of paropakar incomplete and other traces added and the minute and various bhaipari letter tok nibedan added
</commit_message>
<xml_diff>
--- a/ofc/estimates/bhaipari 250000 setidevi mandir/setidevi mandir.xlsx
+++ b/ofc/estimates/bhaipari 250000 setidevi mandir/setidevi mandir.xlsx
@@ -261,10 +261,10 @@
     <t>g/d k|sf/sf] Sn] / l;N6L df6f]df ;j} lsl;dsf] vGg] sfd</t>
   </si>
   <si>
-    <t>Date:2081/09/28</t>
-  </si>
-  <si>
-    <t>Project:- Setidevi mandir</t>
+    <t xml:space="preserve">Project:- सेतीदेवी मन्दिर जाने बाटो निर्माण </t>
+  </si>
+  <si>
+    <t>Date:2081/09/29</t>
   </si>
 </sst>
 </file>
@@ -594,76 +594,76 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -710,8 +710,8 @@
       <sheetName val="PPMO_BOQ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
         <row r="16">
           <cell r="B16" t="str">
             <v>Clearing and Grubbing Road Land ., Clearing and grubbing road land including uprooting rank vegetation, grass, bushes, shrubs, saplings and trees girth up to 300 mm, removal of stumps of trees cut earlier and disposal of unserviceable materials and stacking of serviceable Material to be used or auctioned, up to a lead of 30 meters including removal and disposal of top organic soil not exceeding 150 mm in thickness., By Mechanical Means, In area of light jungle (less than 15 number per 100 sqm )</v>
@@ -753,25 +753,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1303,90 +1303,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
     </row>
     <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="79" t="e">
+      <c r="C6" s="69" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="80"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1394,11 +1394,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="79" t="e">
+      <c r="J6" s="69" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="80"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -1407,77 +1407,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="I7" s="75" t="s">
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="I7" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="70" t="e">
+      <c r="A8" s="77" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="I8" s="76" t="s">
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="I8" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="e">
+      <c r="A9" s="81" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="I9" s="76" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="I9" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="72" t="s">
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="73" t="s">
+      <c r="K11" s="76" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="72"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1496,8 +1496,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="72"/>
-      <c r="K12" s="73"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="76"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="e">
@@ -1659,13 +1659,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1679,6 +1672,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1715,113 +1715,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
     </row>
     <row r="5" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
     </row>
     <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="83" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="88" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="85" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1874,13 +1874,13 @@
       <c r="I9" s="37"/>
       <c r="J9" s="37"/>
       <c r="K9" s="37"/>
-      <c r="M9" s="90" t="s">
+      <c r="M9" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="N9" s="90" t="s">
+      <c r="N9" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="90" t="s">
+      <c r="O9" s="68" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2140,7 +2140,7 @@
       <c r="A19" s="18">
         <v>3</v>
       </c>
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="67" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="19"/>
@@ -2366,7 +2366,7 @@
       <c r="A30" s="18">
         <v>5</v>
       </c>
-      <c r="B30" s="89" t="s">
+      <c r="B30" s="67" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="19"/>
@@ -2762,11 +2762,11 @@
       <c r="B48" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="86">
+      <c r="C48" s="87">
         <f>J46</f>
         <v>282373.23585084308</v>
       </c>
-      <c r="D48" s="86"/>
+      <c r="D48" s="87"/>
       <c r="E48" s="40">
         <v>100</v>
       </c>
@@ -2789,10 +2789,10 @@
       <c r="B49" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="87">
+      <c r="C49" s="90">
         <v>250000</v>
       </c>
-      <c r="D49" s="87"/>
+      <c r="D49" s="90"/>
       <c r="E49" s="40"/>
       <c r="F49" s="50"/>
       <c r="G49" s="49"/>
@@ -2813,11 +2813,11 @@
       <c r="B50" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="87">
+      <c r="C50" s="90">
         <f>C49-C52-C53</f>
         <v>237500</v>
       </c>
-      <c r="D50" s="87"/>
+      <c r="D50" s="90"/>
       <c r="E50" s="40">
         <f>C50/C48*100</f>
         <v>84.108537866334359</v>
@@ -2841,11 +2841,11 @@
       <c r="B51" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="86">
+      <c r="C51" s="87">
         <f>C48-C50</f>
         <v>44873.235850843077</v>
       </c>
-      <c r="D51" s="86"/>
+      <c r="D51" s="87"/>
       <c r="E51" s="40">
         <f>100-E50</f>
         <v>15.891462133665641</v>
@@ -2869,11 +2869,11 @@
       <c r="B52" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="86">
+      <c r="C52" s="87">
         <f>C49*0.03</f>
         <v>7500</v>
       </c>
-      <c r="D52" s="86"/>
+      <c r="D52" s="87"/>
       <c r="E52" s="40">
         <v>3</v>
       </c>
@@ -2896,11 +2896,11 @@
       <c r="B53" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C53" s="86">
+      <c r="C53" s="87">
         <f>C49*0.02</f>
         <v>5000</v>
       </c>
-      <c r="D53" s="86"/>
+      <c r="D53" s="87"/>
       <c r="E53" s="40">
         <v>2</v>
       </c>
@@ -3037,13 +3037,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="A7:F7"/>
@@ -3052,9 +3045,16 @@
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;LPrepared By:
 &amp;CChecked By:
@@ -3102,11 +3102,11 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="88">
+      <c r="C3" s="66">
         <f>(3.917+1.25)/3.281</f>
         <v>1.5748247485522706</v>
       </c>
-      <c r="F3" s="88">
+      <c r="F3" s="66">
         <f>10/12/3.281</f>
         <v>0.25398760540485626</v>
       </c>
@@ -3115,19 +3115,19 @@
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="C4" s="88">
+      <c r="C4" s="66">
         <f>4.5/3.281</f>
         <v>1.3715330691862238</v>
       </c>
-      <c r="D4" s="88">
+      <c r="D4" s="66">
         <f>(C3+C4)/2</f>
         <v>1.4731789088692473</v>
       </c>
-      <c r="E4" s="88">
+      <c r="E4" s="66">
         <f>B4*C4</f>
         <v>6.8576653459311192</v>
       </c>
-      <c r="F4" s="88">
+      <c r="F4" s="66">
         <f>10/12/3.281</f>
         <v>0.25398760540485626</v>
       </c>
@@ -3136,19 +3136,19 @@
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" s="88">
+      <c r="C5" s="66">
         <f>5/3.281</f>
         <v>1.5239256324291375</v>
       </c>
-      <c r="D5" s="88">
+      <c r="D5" s="66">
         <f t="shared" ref="D5:D16" si="0">(C4+C5)/2</f>
         <v>1.4477293508076805</v>
       </c>
-      <c r="E5" s="88">
-        <f t="shared" ref="E5:E16" si="1">B5*C5</f>
+      <c r="E5" s="66">
+        <f t="shared" ref="E5:E15" si="1">B5*C5</f>
         <v>7.6196281621456876</v>
       </c>
-      <c r="F5" s="88">
+      <c r="F5" s="66">
         <f>7/12/3.281</f>
         <v>0.17779132378339937</v>
       </c>
@@ -3157,19 +3157,19 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="88">
+      <c r="C6" s="66">
         <f>5/3.281</f>
         <v>1.5239256324291375</v>
       </c>
-      <c r="D6" s="88">
+      <c r="D6" s="66">
         <f t="shared" si="0"/>
         <v>1.5239256324291375</v>
       </c>
-      <c r="E6" s="88">
+      <c r="E6" s="66">
         <f t="shared" si="1"/>
         <v>7.6196281621456876</v>
       </c>
-      <c r="F6" s="88">
+      <c r="F6" s="66">
         <f>6/12/3.281</f>
         <v>0.15239256324291373</v>
       </c>
@@ -3178,19 +3178,19 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="88">
+      <c r="C7" s="66">
         <f>5.42/3.281</f>
         <v>1.6519353855531849</v>
       </c>
-      <c r="D7" s="88">
+      <c r="D7" s="66">
         <f t="shared" si="0"/>
         <v>1.5879305089911613</v>
       </c>
-      <c r="E7" s="88">
+      <c r="E7" s="66">
         <f t="shared" si="1"/>
         <v>8.2596769277659234</v>
       </c>
-      <c r="F7" s="88">
+      <c r="F7" s="66">
         <v>0</v>
       </c>
     </row>
@@ -3198,19 +3198,19 @@
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" s="88">
+      <c r="C8" s="66">
         <f>6.333/3.281</f>
         <v>1.9302042060347455</v>
       </c>
-      <c r="D8" s="88">
+      <c r="D8" s="66">
         <f t="shared" si="0"/>
         <v>1.7910697957939652</v>
       </c>
-      <c r="E8" s="88">
+      <c r="E8" s="66">
         <f t="shared" si="1"/>
         <v>9.6510210301737267</v>
       </c>
-      <c r="F8" s="88">
+      <c r="F8" s="66">
         <v>0</v>
       </c>
     </row>
@@ -3218,19 +3218,19 @@
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="88">
+      <c r="C9" s="66">
         <f>6.5/3.281</f>
         <v>1.9811033221578787</v>
       </c>
-      <c r="D9" s="88">
+      <c r="D9" s="66">
         <f t="shared" si="0"/>
         <v>1.9556537640963121</v>
       </c>
-      <c r="E9" s="88">
+      <c r="E9" s="66">
         <f t="shared" si="1"/>
         <v>9.9055166107893928</v>
       </c>
-      <c r="F9" s="88">
+      <c r="F9" s="66">
         <v>0</v>
       </c>
     </row>
@@ -3238,19 +3238,19 @@
       <c r="B10">
         <v>5</v>
       </c>
-      <c r="C10" s="88">
+      <c r="C10" s="66">
         <f>7/3.281</f>
         <v>2.1334958854007922</v>
       </c>
-      <c r="D10" s="88">
+      <c r="D10" s="66">
         <f t="shared" si="0"/>
         <v>2.0572996037793354</v>
       </c>
-      <c r="E10" s="88">
+      <c r="E10" s="66">
         <f t="shared" si="1"/>
         <v>10.667479427003961</v>
       </c>
-      <c r="F10" s="88">
+      <c r="F10" s="66">
         <v>0</v>
       </c>
     </row>
@@ -3258,19 +3258,19 @@
       <c r="B11">
         <v>5</v>
       </c>
-      <c r="C11" s="88">
+      <c r="C11" s="66">
         <f>6.5/3.281</f>
         <v>1.9811033221578787</v>
       </c>
-      <c r="D11" s="88">
+      <c r="D11" s="66">
         <f t="shared" si="0"/>
         <v>2.0572996037793354</v>
       </c>
-      <c r="E11" s="88">
+      <c r="E11" s="66">
         <f t="shared" si="1"/>
         <v>9.9055166107893928</v>
       </c>
-      <c r="F11" s="88">
+      <c r="F11" s="66">
         <v>0.05</v>
       </c>
     </row>
@@ -3278,19 +3278,19 @@
       <c r="B12">
         <v>5</v>
       </c>
-      <c r="C12" s="88">
+      <c r="C12" s="66">
         <f>6.5/3.281</f>
         <v>1.9811033221578787</v>
       </c>
-      <c r="D12" s="88">
+      <c r="D12" s="66">
         <f t="shared" si="0"/>
         <v>1.9811033221578787</v>
       </c>
-      <c r="E12" s="88">
+      <c r="E12" s="66">
         <f t="shared" si="1"/>
         <v>9.9055166107893928</v>
       </c>
-      <c r="F12" s="88">
+      <c r="F12" s="66">
         <v>0.05</v>
       </c>
     </row>
@@ -3298,19 +3298,19 @@
       <c r="B13">
         <v>5</v>
       </c>
-      <c r="C13" s="88">
+      <c r="C13" s="66">
         <f>6.75/3.281</f>
         <v>2.0572996037793354</v>
       </c>
-      <c r="D13" s="88">
+      <c r="D13" s="66">
         <f t="shared" si="0"/>
         <v>2.0192014629686073</v>
       </c>
-      <c r="E13" s="88">
+      <c r="E13" s="66">
         <f t="shared" si="1"/>
         <v>10.286498018896676</v>
       </c>
-      <c r="F13" s="88">
+      <c r="F13" s="66">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -3318,19 +3318,19 @@
       <c r="B14">
         <v>5</v>
       </c>
-      <c r="C14" s="88">
+      <c r="C14" s="66">
         <f>7.25/3.281</f>
         <v>2.2096921670222494</v>
       </c>
-      <c r="D14" s="88">
+      <c r="D14" s="66">
         <f t="shared" si="0"/>
         <v>2.1334958854007926</v>
       </c>
-      <c r="E14" s="88">
+      <c r="E14" s="66">
         <f t="shared" si="1"/>
         <v>11.048460835111246</v>
       </c>
-      <c r="F14" s="88">
+      <c r="F14" s="66">
         <v>0</v>
       </c>
     </row>
@@ -3338,19 +3338,19 @@
       <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15" s="88">
+      <c r="C15" s="66">
         <f>7/3.281</f>
         <v>2.1334958854007922</v>
       </c>
-      <c r="D15" s="88">
+      <c r="D15" s="66">
         <f t="shared" si="0"/>
         <v>2.1715940262115208</v>
       </c>
-      <c r="E15" s="88">
+      <c r="E15" s="66">
         <f t="shared" si="1"/>
         <v>10.667479427003961</v>
       </c>
-      <c r="F15" s="88">
+      <c r="F15" s="66">
         <v>0.05</v>
       </c>
     </row>
@@ -3358,26 +3358,26 @@
       <c r="B16">
         <v>2.25</v>
       </c>
-      <c r="C16" s="88">
+      <c r="C16" s="66">
         <f>6.75/3.281</f>
         <v>2.0572996037793354</v>
       </c>
-      <c r="D16" s="88">
+      <c r="D16" s="66">
         <f t="shared" si="0"/>
         <v>2.0953977445900636</v>
       </c>
-      <c r="E16" s="88">
+      <c r="E16" s="66">
         <f>((B16+B15)/2)*C16</f>
         <v>7.4577110637000912</v>
       </c>
-      <c r="F16" s="88">
+      <c r="F16" s="66">
         <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88">
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66">
         <f>SUM(E4:E16)</f>
         <v>119.85179823224627</v>
       </c>
@@ -3387,16 +3387,16 @@
         <f>SUM(B4:B16)</f>
         <v>62.25</v>
       </c>
-      <c r="C18" s="88">
+      <c r="C18" s="66">
         <f>AVERAGE(C3:C16)</f>
         <v>1.8650672704314886</v>
       </c>
-      <c r="D18" s="88">
+      <c r="D18" s="66">
         <f>B18*C18</f>
         <v>116.10043758436017</v>
       </c>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88">
+      <c r="E18" s="66"/>
+      <c r="F18" s="66">
         <f>AVERAGE(F3:F16)</f>
         <v>7.9511364131144693E-2</v>
       </c>

</xml_diff>